<commit_message>
Changes made on page object and excel
</commit_message>
<xml_diff>
--- a/TestData/TestStub.xlsx
+++ b/TestData/TestStub.xlsx
@@ -27,16 +27,16 @@
     <t>EmployeeID</t>
   </si>
   <si>
-    <t>MemoCodes</t>
-  </si>
-  <si>
-    <t>WGPS</t>
-  </si>
-  <si>
-    <t>Deductions</t>
-  </si>
-  <si>
-    <t>WageAgreement,Garnishment</t>
+    <t>Sell</t>
+  </si>
+  <si>
+    <t>Ded</t>
+  </si>
+  <si>
+    <t>Waget,Garnish</t>
+  </si>
+  <si>
+    <t>Shirts</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -387,7 +387,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -398,10 +398,10 @@
         <v>1245</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>